<commit_message>
Iterated over clients file and fixed summary
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\PYCharms\PhoneDivert Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hashir\Desktop\Upwork\Python\PhoneDivert Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B3CA07-0908-43BD-AFED-857AF8A8037B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8840C7-C1A7-42CF-8471-B2FF0E86D244}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,20 +450,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -480,7 +480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -494,7 +494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -508,7 +508,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -522,7 +522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -536,7 +536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -550,7 +550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -564,7 +564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -592,7 +592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -606,7 +606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -620,7 +620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -634,7 +634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -648,7 +648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -662,7 +662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -676,7 +676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -690,7 +690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -704,7 +704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -732,7 +732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -746,7 +746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -760,7 +760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -774,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -788,7 +788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -802,7 +802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -816,7 +816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -830,7 +830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -844,7 +844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -858,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -872,7 +872,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -884,11 +884,6 @@
       </c>
       <c r="E30">
         <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1019064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>